<commit_message>
Initial exploration of annotation
</commit_message>
<xml_diff>
--- a/Structural_elements.xlsx
+++ b/Structural_elements.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jure\Desktop\gnomAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61EEB5A-7FB7-4639-8464-4D3774C84C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E5C4FC5-34D6-40D9-9775-37FE24DDF8C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{305C21C7-1A04-4DBA-9567-462A5CECA9AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Structural_elements" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C37D856-6B35-4E0C-B741-088E4C9F9DFB}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -538,7 +538,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -552,7 +552,7 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -566,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -580,7 +580,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -594,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -636,7 +636,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -650,7 +650,7 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -664,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -678,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
@@ -692,7 +692,7 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -706,7 +706,7 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
@@ -720,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -734,7 +734,7 @@
         <v>15</v>
       </c>
       <c r="C19">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -748,7 +748,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -762,7 +762,7 @@
         <v>16</v>
       </c>
       <c r="C21">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -776,7 +776,7 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -790,7 +790,7 @@
         <v>17</v>
       </c>
       <c r="C23">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
@@ -804,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -818,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -832,7 +832,7 @@
         <v>18</v>
       </c>
       <c r="C26">
-        <v>287</v>
+        <v>311</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
@@ -846,7 +846,7 @@
         <v>19</v>
       </c>
       <c r="C27">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -860,7 +860,7 @@
         <v>20</v>
       </c>
       <c r="C28">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -874,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="C29">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
@@ -888,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="C30">
-        <v>291</v>
+        <v>315</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
@@ -902,7 +902,7 @@
         <v>8</v>
       </c>
       <c r="C31">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
@@ -916,7 +916,7 @@
         <v>20</v>
       </c>
       <c r="C32">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
@@ -930,7 +930,7 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <v>294</v>
+        <v>318</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
@@ -944,7 +944,7 @@
         <v>18</v>
       </c>
       <c r="C34">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
@@ -958,7 +958,7 @@
         <v>17</v>
       </c>
       <c r="C35">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="D35" t="s">
         <v>26</v>
@@ -972,7 +972,7 @@
         <v>20</v>
       </c>
       <c r="C36">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="D36" t="s">
         <v>26</v>
@@ -986,7 +986,7 @@
         <v>8</v>
       </c>
       <c r="C37">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="D37" t="s">
         <v>26</v>
@@ -1000,7 +1000,7 @@
         <v>6</v>
       </c>
       <c r="C38">
-        <v>228</v>
+        <v>255</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
@@ -1014,7 +1014,7 @@
         <v>24</v>
       </c>
       <c r="C39">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -1028,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="C40">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
@@ -1042,7 +1042,7 @@
         <v>17</v>
       </c>
       <c r="C41">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="D41" t="s">
         <v>26</v>
@@ -1056,7 +1056,7 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>232</v>
+        <v>259</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -1070,7 +1070,7 @@
         <v>25</v>
       </c>
       <c r="C43">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -1084,7 +1084,7 @@
         <v>19</v>
       </c>
       <c r="C44">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="D44" t="s">
         <v>26</v>
@@ -1098,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="D45" t="s">
         <v>26</v>
@@ -1112,7 +1112,7 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
@@ -1126,7 +1126,7 @@
         <v>7</v>
       </c>
       <c r="C47">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="D47" t="s">
         <v>26</v>
@@ -1140,7 +1140,7 @@
         <v>8</v>
       </c>
       <c r="C48">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D48" t="s">
         <v>26</v>
@@ -1154,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="D49" t="s">
         <v>26</v>
@@ -1168,7 +1168,7 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="D50" t="s">
         <v>26</v>
@@ -1182,7 +1182,7 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="D51" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Cleaning up and tweaking
</commit_message>
<xml_diff>
--- a/Structural_elements.xlsx
+++ b/Structural_elements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jure\Documents\GitHub\gnomAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jure\Desktop\gnomAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7A250-C2F2-48C2-BAD9-E837F7B46D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E39ECE5-0260-4968-8FDC-2242E7D848B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{305C21C7-1A04-4DBA-9567-462A5CECA9AB}"/>
   </bookViews>
@@ -139,7 +139,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,13 +154,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,12 +176,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -204,9 +196,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pisarna">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +236,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pisarna">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -350,7 +342,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pisarna">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C37D856-6B35-4E0C-B741-088E4C9F9DFB}">
-  <dimension ref="A1:F450"/>
+  <dimension ref="A1:D450"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
-      <selection activeCell="F335" sqref="F335"/>
+      <selection activeCell="G330" sqref="G330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2073,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -2095,7 +2087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>23</v>
       </c>
@@ -2109,7 +2101,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>23</v>
       </c>
@@ -2123,7 +2115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>23</v>
       </c>
@@ -2137,7 +2129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>23</v>
       </c>
@@ -2151,7 +2143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>23</v>
       </c>
@@ -2165,7 +2157,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>23</v>
       </c>
@@ -2179,7 +2171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>23</v>
       </c>
@@ -2193,7 +2185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -2206,9 +2198,8 @@
       <c r="D121" t="s">
         <v>33</v>
       </c>
-      <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>23</v>
       </c>
@@ -2222,7 +2213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>23</v>
       </c>
@@ -2236,7 +2227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>23</v>
       </c>
@@ -2250,7 +2241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -2264,7 +2255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>23</v>
       </c>
@@ -2278,7 +2269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>23</v>
       </c>
@@ -2292,7 +2283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>23</v>
       </c>
@@ -5218,7 +5209,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>23</v>
       </c>
@@ -5232,7 +5223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>23</v>
       </c>
@@ -5246,7 +5237,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>23</v>
       </c>
@@ -5260,7 +5251,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>23</v>
       </c>
@@ -5274,7 +5265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>23</v>
       </c>
@@ -5288,7 +5279,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>23</v>
       </c>
@@ -5302,7 +5293,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>23</v>
       </c>
@@ -5316,7 +5307,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>23</v>
       </c>
@@ -5330,7 +5321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>23</v>
       </c>
@@ -5344,7 +5335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>23</v>
       </c>
@@ -5357,9 +5348,8 @@
       <c r="D346" t="s">
         <v>34</v>
       </c>
-      <c r="E346" s="1"/>
-    </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>23</v>
       </c>
@@ -5373,7 +5363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>23</v>
       </c>
@@ -5387,7 +5377,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>23</v>
       </c>
@@ -5401,7 +5391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>23</v>
       </c>
@@ -5415,7 +5405,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>23</v>
       </c>
@@ -5429,7 +5419,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>23</v>
       </c>

</xml_diff>